<commit_message>
#24 - Update data exporter template, update build script for version numbering
</commit_message>
<xml_diff>
--- a/install/suitecrm-analytics/pentaho-solutions/system/SuiteCRMAnalytics/templates/ExcelTemplateOne.xlsx
+++ b/install/suitecrm-analytics/pentaho-solutions/system/SuiteCRMAnalytics/templates/ExcelTemplateOne.xlsx
@@ -20,15 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">Super Fancy Report</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is Header One</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the dynamic data</t>
+    <t xml:space="preserve">SuiteCRM Analytics</t>
   </si>
 </sst>
 </file>
@@ -38,11 +32,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+  <fonts count="6">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -61,9 +56,18 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -75,14 +79,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF200"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFDC6254"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -120,16 +124,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -149,7 +161,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -158,14 +170,14 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFDC6254"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -213,17 +225,17 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.05"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -231,13 +243,9 @@
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
+    <row r="5" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>